<commit_message>
DOSINZAGE2-445: Updated test data
</commit_message>
<xml_diff>
--- a/test/Testdata_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
+++ b/test/Testdata_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-Images/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633862E0-15CC-D64D-9ED0-4EDFC52D8568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD6088B-B353-1647-A681-BEA7F5309604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19300" xr2:uid="{1650A346-D655-9F40-A836-70310FE71EFF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
   <si>
     <t>Testcase</t>
   </si>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F9EBAD-47C5-D644-9667-952271EB079B}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -928,6 +928,9 @@
       <c r="C2" s="3" t="s">
         <v>56</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1005,6 +1008,9 @@
       <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
@@ -1082,6 +1088,9 @@
       <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="D4" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
@@ -1159,6 +1168,9 @@
       <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
@@ -1236,6 +1248,9 @@
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E6" s="6" t="s">
         <v>14</v>
       </c>
@@ -1393,6 +1408,9 @@
       <c r="C8" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E8" s="6" t="s">
         <v>34</v>
       </c>
@@ -1405,7 +1423,9 @@
       <c r="H8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="J8" s="6">
         <v>6020806</v>
       </c>

</xml_diff>

<commit_message>
DOSINZAGE2-412: Updated StudyInstanceUID in scenario 2.1 and 3.1
</commit_message>
<xml_diff>
--- a/test/Testdata_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
+++ b/test/Testdata_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-Images/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD6088B-B353-1647-A681-BEA7F5309604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E850AF-B4F0-CD43-978B-A5D2F9FCE35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19300" xr2:uid="{1650A346-D655-9F40-A836-70310FE71EFF}"/>
+    <workbookView xWindow="-29260" yWindow="3400" windowWidth="29100" windowHeight="18060" xr2:uid="{1650A346-D655-9F40-A836-70310FE71EFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
   <si>
     <t>Testcase</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>MRI van linker bovenbeen</t>
+  </si>
+  <si>
+    <t>1.2.826.0.1.3680043.8.498.77615907425522706317163091876421984542</t>
+  </si>
+  <si>
+    <t>1.2.826.0.1.3680043.8.498.90783674708684117220863480423356599801</t>
   </si>
 </sst>
 </file>
@@ -803,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F9EBAD-47C5-D644-9667-952271EB079B}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,7 +840,7 @@
     <col min="23" max="23" width="21.5" style="1" customWidth="1"/>
     <col min="24" max="24" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="32.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="62.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
@@ -1075,7 +1081,7 @@
         <v>36</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1395,7 +1401,7 @@
         <v>72</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1496,6 +1502,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100597771DCE5E0DD409E6796B5544574D3" ma:contentTypeVersion="14" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="1f155c61874143f60c84865cea76726f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xmlns:ns3="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7515b2bcca035c7557d524d6ba7a724c" ns2:_="" ns3:_="">
     <xsd:import namespace="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
@@ -1724,15 +1739,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381658C6-125F-4228-83B4-050ACEF74B3B}">
   <ds:schemaRefs>
@@ -1751,6 +1757,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D2DF77-57FD-466E-B6E2-147D6ED80D92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A85AB6D9-DC84-473F-93E0-175F4EA5C2B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1769,14 +1783,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D2DF77-57FD-466E-B6E2-147D6ED80D92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" enabled="0" method="" siteId="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" removed="1"/>

</xml_diff>

<commit_message>
DOSINZAGE2-450: Updated test data
</commit_message>
<xml_diff>
--- a/test/Testdata_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
+++ b/test/Testdata_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-Images/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E850AF-B4F0-CD43-978B-A5D2F9FCE35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9498A88B-3CB2-E242-9760-787C7606575B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29260" yWindow="3400" windowWidth="29100" windowHeight="18060" xr2:uid="{1650A346-D655-9F40-A836-70310FE71EFF}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19180" xr2:uid="{1650A346-D655-9F40-A836-70310FE71EFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="141">
   <si>
     <t>Testcase</t>
   </si>
@@ -56,9 +56,6 @@
     <t>0362 (radiologie)</t>
   </si>
   <si>
-    <t>V6 Algmeen ziekenhuis</t>
-  </si>
-  <si>
     <t>[Leeg]</t>
   </si>
   <si>
@@ -167,24 +164,6 @@
     <t>RAD-20250212-74920</t>
   </si>
   <si>
-    <t>23-05-2024 - 12.00</t>
-  </si>
-  <si>
-    <t>10-02-1990 - 12.00</t>
-  </si>
-  <si>
-    <t>06-02-1993 - 12.00</t>
-  </si>
-  <si>
-    <t>10-08-2020 - 12.00</t>
-  </si>
-  <si>
-    <t>03-03-2020 - 12.00</t>
-  </si>
-  <si>
-    <t>24-05-2024 - 12.00</t>
-  </si>
-  <si>
     <t>Patient.Identificatienumer</t>
   </si>
   <si>
@@ -327,13 +306,166 @@
   </si>
   <si>
     <t>1.2.826.0.1.3680043.8.498.90783674708684117220863480423356599801</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>999990019</t>
+  </si>
+  <si>
+    <t>Patient.Naamgegevens.Initialen</t>
+  </si>
+  <si>
+    <t>B.</t>
+  </si>
+  <si>
+    <t>XXX-Aansluittest-B</t>
+  </si>
+  <si>
+    <t>CR CWK MedMij</t>
+  </si>
+  <si>
+    <t>06011009</t>
+  </si>
+  <si>
+    <t>0361 (radiotherapie)</t>
+  </si>
+  <si>
+    <t>01.010 (Cardioloog)</t>
+  </si>
+  <si>
+    <t>01.015 (Huisarts)</t>
+  </si>
+  <si>
+    <t>113091000 - MRI</t>
+  </si>
+  <si>
+    <t>77477000 - CT</t>
+  </si>
+  <si>
+    <t>44491008 - röntgendoorlichting</t>
+  </si>
+  <si>
+    <t>Catharina Ziekenhuis Eindhoven</t>
+  </si>
+  <si>
+    <t>V6 Algemeen ziekenhuis</t>
+  </si>
+  <si>
+    <t>b7e5d9e2-9e5f-4df6-bc0f-9f98b6d4c705</t>
+  </si>
+  <si>
+    <t>23-05-2024 - 12:00</t>
+  </si>
+  <si>
+    <t>10-02-1990 - 12:00</t>
+  </si>
+  <si>
+    <t>06-02-1993 - 12:00</t>
+  </si>
+  <si>
+    <t>10-08-2020 - 12:00</t>
+  </si>
+  <si>
+    <t>03-03-2020 - 12:00</t>
+  </si>
+  <si>
+    <t>07-08-2024 - 11:57</t>
+  </si>
+  <si>
+    <t>MedMij PGO test MR</t>
+  </si>
+  <si>
+    <t>EXT-14115</t>
+  </si>
+  <si>
+    <t>2.16.840.1.114493.1.4.270.3.20240807115710430</t>
+  </si>
+  <si>
+    <t>a013c0cf-d4f9-4bc5-aa76-ac41347454bd</t>
+  </si>
+  <si>
+    <t>MedMij PGO test CT</t>
+  </si>
+  <si>
+    <t>EXT-14117</t>
+  </si>
+  <si>
+    <t>1.3.12.2.1107.5.1.7.130290.30000024082216430327200000003</t>
+  </si>
+  <si>
+    <t>14206553-b245-4f16-bd9b-78e3b667d879</t>
+  </si>
+  <si>
+    <t>22-08-2024  - 16:45</t>
+  </si>
+  <si>
+    <t>24-05-2024 - 12:00</t>
+  </si>
+  <si>
+    <t>17-01-2025 - 08:44</t>
+  </si>
+  <si>
+    <t>MedMij PGO CT</t>
+  </si>
+  <si>
+    <t>EXT-14114</t>
+  </si>
+  <si>
+    <t>1.3.12.2.1107.5.1.7.130290.30000025011708292397300000003</t>
+  </si>
+  <si>
+    <t>68dc993f-5430-4344-aa9b-a9ba3d9ff099</t>
+  </si>
+  <si>
+    <t>25-02-2025 - 13:56</t>
+  </si>
+  <si>
+    <t>RF Slikfoto's MedMij</t>
+  </si>
+  <si>
+    <t>b72d10a7-ca14-4c54-9711-fc4241c5d840</t>
+  </si>
+  <si>
+    <t>25-02-2025 - 14:24</t>
+  </si>
+  <si>
+    <t>1.2.752.24.7.3059655634.36524</t>
+  </si>
+  <si>
+    <t>63bab3df-700c-4640-906c-b75e5d028437</t>
+  </si>
+  <si>
+    <t>25-02-2025 - 13:53</t>
+  </si>
+  <si>
+    <t>cc9008c2-8a08-457e-a928-c42d43b1efb7</t>
+  </si>
+  <si>
+    <t>25-02-2025 - 14:07</t>
+  </si>
+  <si>
+    <t>1.2.752.24.7.3059655634.36522</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -369,6 +501,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -413,7 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -470,6 +608,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -807,124 +948,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F9EBAD-47C5-D644-9667-952271EB079B}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="1"/>
-    <col min="2" max="2" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="60.83203125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="1"/>
-    <col min="17" max="17" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.5" style="1" customWidth="1"/>
-    <col min="24" max="24" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="62.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="11" style="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="60.83203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" style="1"/>
+    <col min="18" max="18" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.5" style="1" customWidth="1"/>
+    <col min="22" max="22" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.5" style="1" customWidth="1"/>
+    <col min="25" max="25" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="62.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="12" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="12" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="N1" s="12" t="s">
+      <c r="T1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z1" s="12" t="s">
-        <v>73</v>
-      </c>
     </row>
-    <row r="2" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -932,565 +1077,1014 @@
         <v>19056436</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>35178</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="4">
+        <v>45435</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="3">
+        <v>6010713</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4">
-        <v>35178</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="4">
-        <v>45435</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="3">
-        <v>6010713</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="T2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="B3" s="17">
         <v>557807323</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="7">
+        <v>8776</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="7">
-        <v>8776</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="I3" s="7">
+        <v>32914</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="6">
+        <v>6020806</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="7">
-        <v>32914</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="6">
-        <v>6020806</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="M3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" s="6" t="s">
+      <c r="O3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q3" s="6" t="s">
+      <c r="S3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="B4" s="17">
         <v>557807323</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="G4" s="7">
+        <v>8776</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="7">
-        <v>8776</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="I4" s="7">
+        <v>34006</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="6">
+        <v>6020806</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="7">
-        <v>34006</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="6">
-        <v>6020806</v>
-      </c>
-      <c r="K4" s="6" t="s">
+      <c r="M4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="S4" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>45</v>
+        <v>6</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>7</v>
+        <v>112</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>38</v>
+        <v>6</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="17">
         <v>557807323</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="G5" s="7">
+        <v>8776</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="7">
-        <v>8776</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="I5" s="7">
+        <v>34006</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="6">
+        <v>6020806</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="7">
-        <v>34006</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="6">
-        <v>6020806</v>
-      </c>
-      <c r="K5" s="6" t="s">
+      <c r="M5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="O5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="B6" s="17">
         <v>557807323</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="G6" s="7">
+        <v>8776</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="7">
-        <v>8776</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="I6" s="7">
+        <v>44053</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="6">
+        <v>6020806</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="7">
-        <v>44053</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" s="6">
-        <v>6020806</v>
-      </c>
-      <c r="K6" s="6" t="s">
+      <c r="M6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="O6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O6" s="6" t="s">
+      <c r="Q6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q6" s="6" t="s">
+      <c r="S6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="T6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z6" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="B7" s="18">
         <v>120871737</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="4">
+        <v>39448</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="4">
-        <v>39448</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="I7" s="4">
+        <v>43893</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="3">
+        <v>6010754</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="4">
-        <v>43893</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="3">
-        <v>6010754</v>
-      </c>
-      <c r="K7" s="3" t="s">
+      <c r="M7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q7" s="3" t="s">
+      <c r="S7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="U7" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z7" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="B8" s="19">
         <v>267384488</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="G8" s="7">
         <v>36778</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="6">
+        <v>6</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="6">
         <v>6020806</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="L8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="O8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="AA8" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="4">
+        <v>18296</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="4">
+        <v>45511</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="4">
+        <v>18296</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="4">
+        <v>45526</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="4">
+        <v>18296</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="4">
+        <v>45674</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="4">
+        <v>18296</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="4">
+        <v>45674</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>5003249217</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="4">
+        <v>18296</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="4">
+        <v>45674</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>5003249215</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="K9:K11 B9:B13 K12:K13" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
@@ -1499,15 +2093,6 @@
     <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1740,6 +2325,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D2DF77-57FD-466E-B6E2-147D6ED80D92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381658C6-125F-4228-83B4-050ACEF74B3B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1752,14 +2345,6 @@
     <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D2DF77-57FD-466E-B6E2-147D6ED80D92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
DOSINZAGE2-336: Removed test scenario 5.4 in test data and FHIR instances
</commit_message>
<xml_diff>
--- a/test/Testdata_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
+++ b/test/Testdata_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-Images/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9498A88B-3CB2-E242-9760-787C7606575B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF79765-7FE6-D443-B250-508E2F0799ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19180" xr2:uid="{1650A346-D655-9F40-A836-70310FE71EFF}"/>
+    <workbookView xWindow="29560" yWindow="660" windowWidth="34140" windowHeight="27980" xr2:uid="{1650A346-D655-9F40-A836-70310FE71EFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="134">
   <si>
     <t>Testcase</t>
   </si>
@@ -320,9 +320,6 @@
     <t>5.4</t>
   </si>
   <si>
-    <t>5.5</t>
-  </si>
-  <si>
     <t>999990019</t>
   </si>
   <si>
@@ -426,24 +423,6 @@
   </si>
   <si>
     <t>1.3.12.2.1107.5.1.7.130290.30000025011708292397300000003</t>
-  </si>
-  <si>
-    <t>68dc993f-5430-4344-aa9b-a9ba3d9ff099</t>
-  </si>
-  <si>
-    <t>25-02-2025 - 13:56</t>
-  </si>
-  <si>
-    <t>RF Slikfoto's MedMij</t>
-  </si>
-  <si>
-    <t>b72d10a7-ca14-4c54-9711-fc4241c5d840</t>
-  </si>
-  <si>
-    <t>25-02-2025 - 14:24</t>
-  </si>
-  <si>
-    <t>1.2.752.24.7.3059655634.36524</t>
   </si>
   <si>
     <t>63bab3df-700c-4640-906c-b75e5d028437</t>
@@ -948,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F9EBAD-47C5-D644-9667-952271EB079B}">
-  <dimension ref="A1:AA13"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -997,7 +976,7 @@
         <v>43</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>54</v>
@@ -1110,7 +1089,7 @@
         <v>5</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>6</v>
@@ -1131,7 +1110,7 @@
         <v>70</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>83</v>
@@ -1140,7 +1119,7 @@
         <v>71</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>84</v>
@@ -1214,7 +1193,7 @@
         <v>72</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V3" s="7" t="s">
         <v>85</v>
@@ -1306,7 +1285,7 @@
         <v>73</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Y4" s="7" t="s">
         <v>85</v>
@@ -1380,7 +1359,7 @@
         <v>74</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>85</v>
@@ -1389,7 +1368,7 @@
         <v>75</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Y5" s="7" t="s">
         <v>85</v>
@@ -1463,7 +1442,7 @@
         <v>76</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>86</v>
@@ -1472,7 +1451,7 @@
         <v>77</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y6" s="7" t="s">
         <v>86</v>
@@ -1525,7 +1504,7 @@
         <v>5</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>6</v>
@@ -1546,7 +1525,7 @@
         <v>78</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V7" s="4" t="s">
         <v>87</v>
@@ -1655,19 +1634,19 @@
         <v>90</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="G9" s="4">
         <v>18296</v>
@@ -1679,58 +1658,58 @@
         <v>45511</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K9" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="O9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="T9" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="U9" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="V9" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="V9" s="4" t="s">
+      <c r="W9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="W9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z9" s="3" t="s">
+      <c r="AA9" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="AA9" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="17" x14ac:dyDescent="0.2">
@@ -1738,19 +1717,19 @@
         <v>91</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="G10" s="4">
         <v>18296</v>
@@ -1762,58 +1741,58 @@
         <v>45526</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K10" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="O10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N10" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="T10" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="V10" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="U10" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="V10" s="4" t="s">
+      <c r="W10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="W10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="X10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z10" s="3" t="s">
+      <c r="AA10" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="AA10" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="17" x14ac:dyDescent="0.2">
@@ -1821,19 +1800,19 @@
         <v>92</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="G11" s="4">
         <v>18296</v>
@@ -1845,58 +1824,58 @@
         <v>45674</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K11" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="O11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="T11" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="V11" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="V11" s="4" t="s">
+      <c r="W11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z11" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="W11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z11" s="3" t="s">
+      <c r="AA11" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="17" x14ac:dyDescent="0.2">
@@ -1904,19 +1883,19 @@
         <v>93</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="G12" s="4">
         <v>18296</v>
@@ -1928,20 +1907,20 @@
         <v>45674</v>
       </c>
       <c r="J12" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K12" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="O12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1955,114 +1934,31 @@
         <v>6</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T12" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="U12" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="U12" s="4" t="s">
+      <c r="V12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="W12" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="V12" s="4" t="s">
+      <c r="X12" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="W12" s="3" t="s">
+      <c r="Y12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>5003249215</v>
+      </c>
+      <c r="AA12" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="X12" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y12" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z12" s="3">
-        <v>5003249217</v>
-      </c>
-      <c r="AA12" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="4">
-        <v>18296</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="4">
-        <v>45674</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="K13" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="U13" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="V13" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y13" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z13" s="3">
-        <v>5003249215</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2070,21 +1966,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="K9:K11 B9:B13 K12:K13" numberStoredAsText="1"/>
+    <ignoredError sqref="K9:K11 B9:B11 K12 B12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
@@ -2093,6 +1980,15 @@
     <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2325,14 +2221,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D2DF77-57FD-466E-B6E2-147D6ED80D92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381658C6-125F-4228-83B4-050ACEF74B3B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2345,6 +2233,14 @@
     <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D2DF77-57FD-466E-B6E2-147D6ED80D92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>